<commit_message>
building metadata information on the final dataframe
</commit_message>
<xml_diff>
--- a/Projects/M1 and M2/Suppl_info/Metadata_project_M1_M2_final_df.xlsx
+++ b/Projects/M1 and M2/Suppl_info/Metadata_project_M1_M2_final_df.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rubencito/CAS_datascience/ADS_CAS_Bern_2020/Projects/M1 and M2/Suppl_info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BD55F7-F4D6-2344-8C82-DEA61926A631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDCF98A-77A6-AE49-962E-014A38B69D6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9440" yWindow="8120" windowWidth="28040" windowHeight="17440" xr2:uid="{22DAAEB1-AA84-B941-8C52-3CFE025C8641}"/>
+    <workbookView xWindow="5860" yWindow="2560" windowWidth="40860" windowHeight="23100" xr2:uid="{22DAAEB1-AA84-B941-8C52-3CFE025C8641}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>var_name</t>
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>CountryCode</t>
+  </si>
+  <si>
+    <t>StringencyIndex</t>
+  </si>
+  <si>
+    <t>Country_Region</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>Deaths</t>
+  </si>
+  <si>
+    <t>Recovered</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>New_cases</t>
+  </si>
+  <si>
+    <t>New_deaths</t>
+  </si>
+  <si>
+    <t>New_recovered</t>
+  </si>
+  <si>
+    <t>Confirmed_100K</t>
+  </si>
+  <si>
+    <t>Deaths_100K</t>
+  </si>
+  <si>
+    <t>Recovered_100K</t>
+  </si>
+  <si>
+    <t>Active_100K</t>
+  </si>
+  <si>
+    <t>New_cases_100K</t>
+  </si>
+  <si>
+    <t>New_deaths_100K</t>
+  </si>
+  <si>
+    <t>New_recovered_100K</t>
+  </si>
+  <si>
+    <t>GDP_in_USD</t>
+  </si>
+  <si>
+    <t>incomeLevel.value</t>
+  </si>
+  <si>
+    <t>timestamp in format YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>standart ISO country code nomenclature of 3 characters</t>
+  </si>
+  <si>
+    <t>geverment response indicator for the covid prevention. More info on how this value is calculated can be found in the metadat form Oxford University</t>
+  </si>
+  <si>
+    <t>Country name</t>
+  </si>
+  <si>
+    <t>total population taken from the metadata on Covid data source repository. More info in the JH repository metadata location</t>
+  </si>
+  <si>
+    <t>confirmed cases of covid infections</t>
+  </si>
+  <si>
+    <t>confirmed deaths cases caused by covid infections</t>
+  </si>
+  <si>
+    <t>current active cases of covid infections. Calculated by subtracting Recovered and Death cases to Confirmed cases</t>
+  </si>
+  <si>
+    <t>lag difference of confirmed cases in day-by-day-basis</t>
+  </si>
+  <si>
+    <t>lag difference of death cases in day-by-day-basis</t>
+  </si>
+  <si>
+    <t>lag difference of recovered cases in day-by-day-basis</t>
+  </si>
+  <si>
+    <t>confirmed cases normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>death cases normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>recovered cases normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>active cases normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>new cases normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>new death normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>new recovered normalized by 100000 people</t>
+  </si>
+  <si>
+    <t>Gross domestic product of the country in USD currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income level assigned to the country from the world bank in categorical  </t>
   </si>
 </sst>
 </file>
@@ -382,13 +505,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620F5E9D-A226-D041-A6B2-1265FA2F67B1}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="231" zoomScaleNormal="231" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -398,6 +525,174 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>